<commit_message>
launch senior manager to complete filling amdin
</commit_message>
<xml_diff>
--- a/output/ProviderLogins.xlsx
+++ b/output/ProviderLogins.xlsx
@@ -12,108 +12,132 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
-  <si>
-    <t>provider200</t>
-  </si>
-  <si>
-    <t>provider201</t>
-  </si>
-  <si>
-    <t>provider202</t>
-  </si>
-  <si>
-    <t>provider203</t>
-  </si>
-  <si>
-    <t>provider204</t>
-  </si>
-  <si>
-    <t>provider205</t>
-  </si>
-  <si>
-    <t>provider206</t>
-  </si>
-  <si>
-    <t>provider207</t>
-  </si>
-  <si>
-    <t>provider208</t>
-  </si>
-  <si>
-    <t>provider209</t>
-  </si>
-  <si>
-    <t>provider210</t>
-  </si>
-  <si>
-    <t>provider211</t>
-  </si>
-  <si>
-    <t>provider212</t>
-  </si>
-  <si>
-    <t>provider213</t>
-  </si>
-  <si>
-    <t>provider214</t>
-  </si>
-  <si>
-    <t>provider215</t>
-  </si>
-  <si>
-    <t>provider216</t>
-  </si>
-  <si>
-    <t>provider217</t>
-  </si>
-  <si>
-    <t>provider218</t>
-  </si>
-  <si>
-    <t>provider219</t>
-  </si>
-  <si>
-    <t>provider220</t>
-  </si>
-  <si>
-    <t>provider221</t>
-  </si>
-  <si>
-    <t>provider222</t>
-  </si>
-  <si>
-    <t>provider223</t>
-  </si>
-  <si>
-    <t>provider224</t>
-  </si>
-  <si>
-    <t>provider225</t>
-  </si>
-  <si>
-    <t>provider226</t>
-  </si>
-  <si>
-    <t>provider227</t>
-  </si>
-  <si>
-    <t>provider228</t>
-  </si>
-  <si>
-    <t>provider229</t>
-  </si>
-  <si>
-    <t>provider230</t>
-  </si>
-  <si>
-    <t>provider231</t>
-  </si>
-  <si>
-    <t>provider232</t>
-  </si>
-  <si>
-    <t>provider233</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+  <si>
+    <t>provider500</t>
+  </si>
+  <si>
+    <t>provider501</t>
+  </si>
+  <si>
+    <t>provider502</t>
+  </si>
+  <si>
+    <t>provider503</t>
+  </si>
+  <si>
+    <t>provider504</t>
+  </si>
+  <si>
+    <t>provider505</t>
+  </si>
+  <si>
+    <t>provider506</t>
+  </si>
+  <si>
+    <t>provider507</t>
+  </si>
+  <si>
+    <t>provider508</t>
+  </si>
+  <si>
+    <t>provider509</t>
+  </si>
+  <si>
+    <t>provider510</t>
+  </si>
+  <si>
+    <t>provider511</t>
+  </si>
+  <si>
+    <t>provider512</t>
+  </si>
+  <si>
+    <t>provider513</t>
+  </si>
+  <si>
+    <t>provider514</t>
+  </si>
+  <si>
+    <t>provider515</t>
+  </si>
+  <si>
+    <t>provider516</t>
+  </si>
+  <si>
+    <t>provider517</t>
+  </si>
+  <si>
+    <t>provider518</t>
+  </si>
+  <si>
+    <t>provider519</t>
+  </si>
+  <si>
+    <t>provider520</t>
+  </si>
+  <si>
+    <t>provider521</t>
+  </si>
+  <si>
+    <t>provider522</t>
+  </si>
+  <si>
+    <t>provider523</t>
+  </si>
+  <si>
+    <t>provider524</t>
+  </si>
+  <si>
+    <t>provider525</t>
+  </si>
+  <si>
+    <t>provider526</t>
+  </si>
+  <si>
+    <t>provider527</t>
+  </si>
+  <si>
+    <t>provider528</t>
+  </si>
+  <si>
+    <t>provider529</t>
+  </si>
+  <si>
+    <t>provider530</t>
+  </si>
+  <si>
+    <t>provider531</t>
+  </si>
+  <si>
+    <t>provider532</t>
+  </si>
+  <si>
+    <t>provider533</t>
+  </si>
+  <si>
+    <t>provider534</t>
+  </si>
+  <si>
+    <t>provider535</t>
+  </si>
+  <si>
+    <t>provider536</t>
+  </si>
+  <si>
+    <t>provider537</t>
+  </si>
+  <si>
+    <t>provider538</t>
+  </si>
+  <si>
+    <t>provider539</t>
+  </si>
+  <si>
+    <t>provider540</t>
+  </si>
+  <si>
+    <t>provider541</t>
   </si>
 </sst>
 </file>
@@ -334,6 +358,46 @@
         <v>33</v>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixes in Add Provider
</commit_message>
<xml_diff>
--- a/output/ProviderLogins.xlsx
+++ b/output/ProviderLogins.xlsx
@@ -14,37 +14,37 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>provider1021</t>
+    <t>provider11</t>
   </si>
   <si>
-    <t>provider1022</t>
+    <t>provider12</t>
   </si>
   <si>
-    <t>provider1023</t>
+    <t>provider13</t>
   </si>
   <si>
-    <t>provider1024</t>
+    <t>provider14</t>
   </si>
   <si>
-    <t>provider1025</t>
+    <t>provider15</t>
   </si>
   <si>
-    <t>provider1026</t>
+    <t>provider16</t>
   </si>
   <si>
-    <t>provider1027</t>
+    <t>provider17</t>
   </si>
   <si>
-    <t>provider1028</t>
+    <t>provider18</t>
   </si>
   <si>
-    <t>provider1029</t>
+    <t>provider19</t>
   </si>
   <si>
-    <t>provider1030</t>
+    <t>provider20</t>
   </si>
   <si>
-    <t>provider1031</t>
+    <t>provider21</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
fixes in AdminAddBrand (rid out file extension)
</commit_message>
<xml_diff>
--- a/output/ProviderLogins.xlsx
+++ b/output/ProviderLogins.xlsx
@@ -14,37 +14,37 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>provider11</t>
+    <t>provider21</t>
   </si>
   <si>
-    <t>provider12</t>
+    <t>provider22</t>
   </si>
   <si>
-    <t>provider13</t>
+    <t>provider23</t>
   </si>
   <si>
-    <t>provider14</t>
+    <t>provider24</t>
   </si>
   <si>
-    <t>provider15</t>
+    <t>provider25</t>
   </si>
   <si>
-    <t>provider16</t>
+    <t>provider26</t>
   </si>
   <si>
-    <t>provider17</t>
+    <t>provider27</t>
   </si>
   <si>
-    <t>provider18</t>
+    <t>provider28</t>
   </si>
   <si>
-    <t>provider19</t>
+    <t>provider29</t>
   </si>
   <si>
-    <t>provider20</t>
+    <t>provider30</t>
   </si>
   <si>
-    <t>provider21</t>
+    <t>provider31</t>
   </si>
 </sst>
 </file>

</xml_diff>